<commit_message>
obtention d'une liste de dictionnaires pour les données de chaque année (fusion_old_new_data)
</commit_message>
<xml_diff>
--- a/assets/Historique-Indicateurs-Quadri.xlsx
+++ b/assets/Historique-Indicateurs-Quadri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacqu\PycharmProjects\projet cassiopée\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B52AF28-00C0-4483-AB2A-09FCC6362D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4274C525-085A-4478-A214-E86D2AE37D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="41">
   <si>
     <t>Année</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Thèses</t>
+  </si>
+  <si>
+    <t>Non-permanents recherche en ETPT (base annuelle)</t>
   </si>
 </sst>
 </file>
@@ -598,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3046,7 +3049,7 @@
   <dimension ref="A1:AI28"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4826,7 +4829,7 @@
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
         <v>27</v>

</xml_diff>